<commit_message>
replace the new excel file
</commit_message>
<xml_diff>
--- a/encode-nero-ffmpeg-mkv.xlsx
+++ b/encode-nero-ffmpeg-mkv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Documents 3\Encoder Command\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Documents 3\Encoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6489B40-6A57-4293-86E1-656690FD13E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D193CB98-0162-49C2-9B31-E62B1E0B4E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="642" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="161">
   <si>
     <t>ffmpeg -i</t>
   </si>
@@ -74,9 +74,6 @@
     <t>open cmd</t>
   </si>
   <si>
-    <t>cd "directory"</t>
-  </si>
-  <si>
     <t>-br 32000</t>
   </si>
   <si>
@@ -290,27 +287,6 @@
     <t>VHS - Stella Interview (Machine Room).mp4</t>
   </si>
   <si>
-    <t>https://www.codegrepper.com/code-examples/shell/ffmpeg+convert+to+mp4</t>
-  </si>
-  <si>
-    <t>[FFMPEG resolution helper]</t>
-  </si>
-  <si>
-    <t>mkvmerge</t>
-  </si>
-  <si>
-    <t>mkvextract</t>
-  </si>
-  <si>
-    <t>[mkvtoolnix]</t>
-  </si>
-  <si>
-    <t>ffmpeg -i "somevideo.h264" -i "someaudio.mp3" -c:v copy -c:a copy -map_metadata -1 -movflags +faststart -y "something.mp4"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ffmpeg -i vid.avc -i 1.flac -c:v copy -c:a copy -strict -2 1.mp4 </t>
-  </si>
-  <si>
     <t>F:\</t>
   </si>
   <si>
@@ -431,15 +407,9 @@
     <t>E:\temp\</t>
   </si>
   <si>
-    <t>temp</t>
-  </si>
-  <si>
     <t>MIX</t>
   </si>
   <si>
-    <t>create folder !</t>
-  </si>
-  <si>
     <t>END</t>
   </si>
   <si>
@@ -495,13 +465,121 @@
   </si>
   <si>
     <t>[mentoring]akm 1 UAS.mp4 - Google Drive_2.mp4</t>
+  </si>
+  <si>
+    <t>cd &lt;directory_of_your_videos&gt;</t>
+  </si>
+  <si>
+    <t>open file.txt</t>
+  </si>
+  <si>
+    <t>copy video name and format</t>
+  </si>
+  <si>
+    <t>paste video name and format in the A column</t>
+  </si>
+  <si>
+    <t>create the folder first !</t>
+  </si>
+  <si>
+    <t>output folder :</t>
+  </si>
+  <si>
+    <t>change the output directory in L5 (column L ; row 5)</t>
+  </si>
+  <si>
+    <t>go to file explorer directory_of_your_videos</t>
+  </si>
+  <si>
+    <t>edit file.txt and paste it</t>
+  </si>
+  <si>
+    <t>change file.txt to file.cmd</t>
+  </si>
+  <si>
+    <t>execute it</t>
+  </si>
+  <si>
+    <t>go to AE1, copy all column AE (right of "MIX")</t>
+  </si>
+  <si>
+    <t>ffmpeg</t>
+  </si>
+  <si>
+    <t>mkvtoolnix</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">YOU NEED TO INSTALL AND ADD THEM TO </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PATH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ---------&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>wait and done :)</t>
+  </si>
+  <si>
+    <t>lol</t>
+  </si>
+  <si>
+    <t>what the heck is this</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">open </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>neroaac4-del_temp_keep_ori</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet (in this excel)</t>
+    </r>
+  </si>
+  <si>
+    <t>Guide :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,6 +595,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -571,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -582,6 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,6 +685,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>311235</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>117231</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>185387</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9363E752-9BC3-447B-BA07-2A0A630D6865}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3960043" y="0"/>
+          <a:ext cx="3454803" cy="1709387"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,70 +1000,130 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EEA341-DB57-4E40-A6CC-00857B13DF2F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:R15"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="R1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>88</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -963,7 +1160,7 @@
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -998,7 +1195,7 @@
         <v>4</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U1" t="str">
         <f>IF(A1&lt;&gt;0,_xlfn.CONCAT($R$1," ",$R$3," ",$R$4," -if ",H1," -of ",I1),"")</f>
@@ -1018,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="AK1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>4</v>
@@ -1038,7 +1235,7 @@
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -1099,7 +1296,7 @@
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -1131,7 +1328,7 @@
         <v>4</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U3" t="str">
         <f t="shared" si="6"/>
@@ -1163,7 +1360,7 @@
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -1195,7 +1392,7 @@
         <v>4</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U4" t="str">
         <f t="shared" si="6"/>
@@ -1219,7 +1416,7 @@
         <v>4</v>
       </c>
       <c r="AR4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AV4" s="1" t="s">
         <v>4</v>
@@ -1227,7 +1424,7 @@
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -1285,7 +1482,7 @@
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -1343,7 +1540,7 @@
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -2511,7 +2708,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:BH40"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AR1" sqref="AR1"/>
     </sheetView>
   </sheetViews>
@@ -2545,7 +2742,7 @@
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -2586,7 +2783,7 @@
         <v>4</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W1" t="str">
         <f t="shared" ref="W1:W40" si="3">IF(A1&lt;&gt;0,_xlfn.CONCAT($T$1," ",$T$3," ",$T$4," -if ","""",$M$3,J1,""""," -of ","""",$M$3,K1,""""),"")</f>
@@ -2606,7 +2803,7 @@
         <v>4</v>
       </c>
       <c r="AM1" s="7" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="AN1" t="str">
         <f>_xlfn.CONCAT("echo. &amp;&amp; echo Delete original file ? &amp;&amp; pause &amp;&amp; pause"," &amp;&amp; ",IF(A1&lt;&gt;0,_xlfn.CONCAT("del ","""",A1,""""," &amp;&amp; del ","""",$M$3,J1,""""," &amp;&amp; del ","""",$M$3,K1,""""),""))</f>
@@ -2627,7 +2824,7 @@
         <v>4</v>
       </c>
       <c r="AW1" s="7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="AX1" t="s">
         <v>8</v>
@@ -2638,7 +2835,7 @@
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -2713,7 +2910,7 @@
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -2744,7 +2941,7 @@
         <v>3.aac</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" si="2"/>
@@ -2754,7 +2951,7 @@
         <v>4</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W3" t="str">
         <f t="shared" si="3"/>
@@ -2794,7 +2991,7 @@
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -2832,7 +3029,7 @@
         <v>4</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W4" t="str">
         <f t="shared" si="3"/>
@@ -2867,12 +3064,12 @@
         <v>4</v>
       </c>
       <c r="AX4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -2944,7 +3141,7 @@
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -3016,7 +3213,7 @@
     </row>
     <row r="7" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -3088,7 +3285,7 @@
     </row>
     <row r="8" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -3160,7 +3357,7 @@
     </row>
     <row r="9" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -3232,7 +3429,7 @@
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -3304,7 +3501,7 @@
     </row>
     <row r="11" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -3376,7 +3573,7 @@
     </row>
     <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
@@ -3448,7 +3645,7 @@
     </row>
     <row r="13" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
@@ -3520,7 +3717,7 @@
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -3592,7 +3789,7 @@
     </row>
     <row r="15" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -3664,7 +3861,7 @@
     </row>
     <row r="16" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -3736,7 +3933,7 @@
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
@@ -3808,7 +4005,7 @@
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -3880,7 +4077,7 @@
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -3952,7 +4149,7 @@
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
@@ -4024,7 +4221,7 @@
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -4096,7 +4293,7 @@
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -4168,7 +4365,7 @@
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>4</v>
@@ -4240,7 +4437,7 @@
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
@@ -4312,7 +4509,7 @@
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>
@@ -4384,7 +4581,7 @@
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>4</v>
@@ -4456,7 +4653,7 @@
     </row>
     <row r="27" spans="1:48" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>4</v>
@@ -4531,7 +4728,7 @@
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -4585,7 +4782,7 @@
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
@@ -4639,7 +4836,7 @@
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -5242,7 +5439,7 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -5283,7 +5480,7 @@
         <v>4</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R1" t="str">
         <f t="shared" ref="R1:R40" si="4">IF(A1&lt;&gt;0,_xlfn.CONCAT($P$1," ",$P$3," ",$P$4," -if ","""",$L$3,I1,""""," -of ","""",$L$3,J1,""""),"")</f>
@@ -5303,7 +5500,7 @@
         <v>4</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="Y1" t="str">
         <f>_xlfn.CONCAT("echo. &amp;&amp; echo Delete temp file ? &amp;&amp; pause &amp;&amp; pause"," &amp;&amp; ",IF(A1&lt;&gt;0,_xlfn.CONCAT("del ","""",$L$3,I1,""""," &amp;&amp; del ","""",$L$3,J1,""""),""))</f>
@@ -5313,7 +5510,7 @@
         <v>4</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="AB1" t="str">
         <f>_xlfn.CONCAT("echo. &amp;&amp; echo DONE!!! &amp;&amp; pause")</f>
@@ -5325,7 +5522,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -5389,7 +5586,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -5420,7 +5617,7 @@
         <v>3.aac</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="N3" t="str">
         <f t="shared" si="3"/>
@@ -5430,7 +5627,7 @@
         <v>4</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" si="4"/>
@@ -5454,12 +5651,12 @@
         <v>4</v>
       </c>
       <c r="AB3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -5497,7 +5694,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="4"/>
@@ -5523,7 +5720,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -5584,7 +5781,7 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -5645,7 +5842,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -5706,7 +5903,7 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -5767,7 +5964,7 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -5828,7 +6025,7 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -5889,7 +6086,7 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -5950,7 +6147,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -6011,7 +6208,7 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -6072,7 +6269,7 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -6133,7 +6330,7 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -6194,7 +6391,7 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -6255,7 +6452,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
@@ -6316,7 +6513,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -8062,8 +8259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFC5F25-8D01-484E-9A5E-FE0D9C7B3A26}">
   <dimension ref="A1:AW60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8076,6 +8273,7 @@
     <col min="8" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7.7109375" customWidth="1"/>
     <col min="11" max="11" width="2.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.140625" customWidth="1"/>
     <col min="14" max="14" width="44.85546875" customWidth="1"/>
     <col min="15" max="15" width="2.5703125" style="1" customWidth="1"/>
@@ -8100,7 +8298,7 @@
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -8144,7 +8342,7 @@
         <v>4</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R1" t="str">
         <f t="shared" ref="R1:R32" si="4">IF(A1&lt;&gt;0,_xlfn.CONCAT($P$1," ",$P$3," ",$P$4," -if ","""",$L$5,I1,""""," -of ","""",$L$5,J1,""""),"")</f>
@@ -8154,7 +8352,7 @@
         <v>4</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="U1" t="str">
         <f t="shared" ref="U1:U32" si="5">_xlfn.CONCAT("del ","""",$L$5,I1,"""")</f>
@@ -8174,7 +8372,7 @@
         <v>4</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="AB1" t="str">
         <f t="shared" ref="AB1:AB32" si="7">_xlfn.CONCAT("del ","""",$L$5,J1,"""")</f>
@@ -8184,7 +8382,7 @@
         <v>4</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AE1" t="str">
         <f>IF(A1&lt;&gt;0,_xlfn.CONCAT(N1," &amp;&amp; ",R1," &amp;&amp; ",U1," &amp;&amp; ",Y1," &amp;&amp; ",AB1),"")</f>
@@ -8194,7 +8392,7 @@
         <v>4</v>
       </c>
       <c r="AN1" s="6" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="AO1" t="str">
         <f>_xlfn.CONCAT("echo. &amp;&amp; echo DONE!!! &amp;&amp; pause")</f>
@@ -8206,7 +8404,7 @@
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -8284,7 +8482,7 @@
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -8318,7 +8516,7 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="M3" t="s">
         <v>4</v>
@@ -8331,7 +8529,7 @@
         <v>4</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" si="4"/>
@@ -8371,7 +8569,7 @@
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -8405,7 +8603,7 @@
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="M4" t="s">
         <v>4</v>
@@ -8418,7 +8616,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="4"/>
@@ -8458,7 +8656,7 @@
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -8492,7 +8690,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M5" t="s">
         <v>4</v>
@@ -8542,7 +8740,7 @@
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -8620,7 +8818,7 @@
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -8698,7 +8896,7 @@
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -8851,7 +9049,7 @@
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -8929,7 +9127,7 @@
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -9007,7 +9205,7 @@
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -9160,7 +9358,7 @@
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -9238,7 +9436,7 @@
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -9391,7 +9589,7 @@
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
@@ -9469,7 +9667,7 @@
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -9547,7 +9745,7 @@
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
@@ -12754,7 +12952,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -12823,7 +13021,7 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -12880,7 +13078,7 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -12937,7 +13135,7 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -12989,12 +13187,12 @@
         <v>4</v>
       </c>
       <c r="X4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -13048,7 +13246,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -13102,7 +13300,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -13156,7 +13354,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -13210,7 +13408,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -13264,7 +13462,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -13318,7 +13516,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -13372,7 +13570,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -14212,7 +14410,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -14222,19 +14420,19 @@
         <v>"[Koenime] Oregairu S1 BD - 01 (1080p).mkv"</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" t="str">
         <f>_xlfn.CONCAT("mkvextract ",C1," attachments 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 24 25 26 27 28 29 30 31 32 33 34 35 36 37 38 39 40 41 42 43 44 45 46 47 48 49 50")</f>
         <v>mkvextract "[Koenime] Oregairu S1 BD - 01 (1080p).mkv" attachments 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 24 25 26 27 28 29 30 31 32 33 34 35 36 37 38 39 40 41 42 43 44 45 46 47 48 49 50</v>
       </c>
       <c r="AH1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -14250,7 +14448,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -14266,7 +14464,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -14282,7 +14480,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -14298,7 +14496,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -14314,7 +14512,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -14330,7 +14528,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -14346,7 +14544,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -14362,7 +14560,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -14378,7 +14576,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -14394,7 +14592,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -14410,7 +14608,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -14426,7 +14624,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -14460,7 +14658,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -14470,22 +14668,22 @@
         <v>"[Koenime] Oregairu S1 BD - 01 (1080p).mkv"</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" t="str">
         <f>_xlfn.CONCAT("mkvmerge -o new/",C1," -M ",C1," ",$H$1)</f>
         <v>mkvmerge -o new/"[Koenime] Oregairu S1 BD - 01 (1080p).mkv" -M "[Koenime] Oregairu S1 BD - 01 (1080p).mkv" font.mkv</v>
       </c>
       <c r="Y1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -14501,7 +14699,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -14517,7 +14715,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -14533,7 +14731,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -14549,7 +14747,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -14565,7 +14763,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -14581,7 +14779,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -14597,7 +14795,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -14613,7 +14811,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -14629,7 +14827,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -14645,7 +14843,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -14661,7 +14859,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -14677,7 +14875,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -14699,7 +14897,7 @@
   <dimension ref="A1:AL28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14711,7 +14909,7 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -14730,7 +14928,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -14746,7 +14944,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -14762,7 +14960,7 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -14778,7 +14976,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -14794,7 +14992,7 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -14810,7 +15008,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -14826,7 +15024,7 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -14842,7 +15040,7 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -14858,7 +15056,7 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -14874,7 +15072,7 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -14890,7 +15088,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -14906,7 +15104,7 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -14922,7 +15120,7 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -14938,7 +15136,7 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -14954,7 +15152,7 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -14970,7 +15168,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -14986,7 +15184,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -15002,7 +15200,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -15018,7 +15216,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -15034,7 +15232,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
@@ -15050,7 +15248,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -15066,7 +15264,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
@@ -15082,7 +15280,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
@@ -15098,7 +15296,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -15114,7 +15312,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -15130,7 +15328,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -15146,7 +15344,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>

</xml_diff>